<commit_message>
text re-writing, adding diagrams
</commit_message>
<xml_diff>
--- a/assets/GPT-lite-cpp/benchmark.xlsx
+++ b/assets/GPT-lite-cpp/benchmark.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-bmagalhaes\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t-bmagalhaes\Desktop\brunomaga.github.io\assets\GPT-lite-cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522D5D37-B630-4053-9475-AF43F0FD9CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5348D29F-7EEB-4878-8667-073988A6BC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11790" yWindow="0" windowWidth="10860" windowHeight="14410" xr2:uid="{AE0F995E-40A1-4209-BC5D-1DA4A89ACD57}"/>
+    <workbookView xWindow="-7430" yWindow="-20460" windowWidth="28800" windowHeight="15910" xr2:uid="{AE0F995E-40A1-4209-BC5D-1DA4A89ACD57}"/>
   </bookViews>
   <sheets>
     <sheet name="benchmark" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="15">
   <si>
     <t>C++</t>
   </si>
@@ -66,13 +66,7 @@
     <t>Pytorch 2.1</t>
   </si>
   <si>
-    <t>cmake .. -DCMAKE_BUILD_TYPE=Release -DCAFFE2_USE_CUSPARSELT=1</t>
-  </si>
-  <si>
     <t>branch use_input_generating_functions</t>
-  </si>
-  <si>
-    <t>pip install torch==1.13.1 torchvision==0.14.1 torchaudio==0.13.1</t>
   </si>
   <si>
     <t>memory usage GB</t>
@@ -137,13 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,7 +474,7 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,17 +489,17 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>15</v>
+      <c r="B1" t="s">
+        <v>13</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -542,7 +535,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>6.35</v>
@@ -561,17 +554,17 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -607,7 +600,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>4.34</v>
@@ -626,17 +619,17 @@
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
+      <c r="B11" t="s">
+        <v>13</v>
       </c>
       <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -672,7 +665,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>10.81</v>
@@ -687,15 +680,8 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A17" s="2"/>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" s="2"/>
@@ -837,7 +823,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>